<commit_message>
EPBDS-7552 - disabled range indexes, equals indexes have higher priority, arrange equals indexes by unique conditions
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7684.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7684.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{66B5CDFE-29C4-4077-B20A-F7E355EE7602}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35F3320-33DA-4BCF-A31F-D6579F5142AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26640" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="4" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>age &gt; minAge &amp;&amp; age &lt;= maxAge</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Test merged  mergedTest</t>
+  </si>
+  <si>
+    <t>(minAge == null || age &gt; minAge) &amp;&amp; (maxAge == null || age &lt;= maxAge)</t>
   </si>
 </sst>
 </file>
@@ -368,18 +368,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% — акцент1" xfId="6" builtinId="30" customBuiltin="1"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,10 +770,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -800,18 +800,18 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="6" t="s">
         <v>3</v>
       </c>
@@ -820,10 +820,10 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="16"/>
+      <c r="B12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="14"/>
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
@@ -912,19 +912,19 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>3</v>
@@ -944,7 +944,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1028,46 +1028,46 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="B33" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="F34" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="E35" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" s="10">
         <v>1</v>
@@ -1095,7 +1095,7 @@
         <v>12</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="10">
         <v>1</v>
@@ -1183,7 +1183,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F42" s="10">
         <v>7</v>
@@ -1200,7 +1200,7 @@
         <v>5</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F43" s="10">
         <v>7</v>
@@ -1217,7 +1217,7 @@
         <v>5</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F44" s="10">
         <v>7</v>
@@ -1231,7 +1231,7 @@
         <v>13</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45" s="10">
         <v>1</v>
@@ -1248,7 +1248,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E46" s="10">
         <v>1</v>
@@ -1336,7 +1336,7 @@
         <v>5</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F51" s="10">
         <v>8</v>
@@ -1373,46 +1373,46 @@
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
+      <c r="B55" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="F56" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="D57" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="E57" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
         <v>12</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E58" s="10">
         <v>1</v>
@@ -1440,7 +1440,7 @@
         <v>12</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E59" s="10">
         <v>1</v>
@@ -1528,7 +1528,7 @@
         <v>5</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F64" s="10">
         <v>7</v>
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F65" s="10">
         <v>7</v>
@@ -1562,7 +1562,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F66" s="10">
         <v>7</v>
@@ -1576,7 +1576,7 @@
         <v>13</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E67" s="10">
         <v>1</v>
@@ -1593,7 +1593,7 @@
         <v>13</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E68" s="10">
         <v>1</v>
@@ -1681,7 +1681,7 @@
         <v>5</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F73" s="10">
         <v>8</v>
@@ -1719,13 +1719,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B33:F33"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B33:F33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
EPBDS-7552 combined range indexes
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7684.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7684.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35F3320-33DA-4BCF-A31F-D6579F5142AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15027E8D-F928-45A9-96A7-2BFFF84A67F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>Test merged  mergedTest</t>
   </si>
   <si>
-    <t>(minAge == null || age &gt; minAge) &amp;&amp; (maxAge == null || age &lt;= maxAge)</t>
+    <t>age &gt; minAge &amp;&amp; age &lt;= maxAge</t>
   </si>
 </sst>
 </file>
@@ -368,18 +368,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% — акцент1" xfId="6" builtinId="30" customBuiltin="1"/>
@@ -755,7 +755,7 @@
   <dimension ref="B3:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,10 +770,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -800,18 +800,18 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="6" t="s">
         <v>3</v>
       </c>
@@ -820,10 +820,10 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
@@ -912,12 +912,12 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
@@ -1028,13 +1028,13 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
@@ -1373,13 +1373,13 @@
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">

</xml_diff>